<commit_message>
Adjust the predicted vs actual plots
</commit_message>
<xml_diff>
--- a/Replication Package/Code and Data/(2) Regressions/Output Data Python (New Model)/summary_stats_new_model.xlsx
+++ b/Replication Package/Code and Data/(2) Regressions/Output Data Python (New Model)/summary_stats_new_model.xlsx
@@ -633,8 +633,12 @@
       <c r="B2" t="n">
         <v>0.5726228392444359</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>3.072906383865932e-05</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0002217231224067183</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -645,8 +649,12 @@
       <c r="B3" t="n">
         <v>4.088055924830122</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>0.310481901381304</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.134853793981501e-05</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -657,8 +665,12 @@
       <c r="B4" t="n">
         <v>3.959255145789188</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>5.633554804655667e-05</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.439655649403873e-08</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>

</xml_diff>